<commit_message>
add logic to check for # in employee number
</commit_message>
<xml_diff>
--- a/07-07-24 to 07-13-24 Milwaukee Schedule Copy.xlsx
+++ b/07-07-24 to 07-13-24 Milwaukee Schedule Copy.xlsx
@@ -4158,8 +4158,16 @@
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr"/>
       <c r="L72" t="inlineStr"/>
-      <c r="M72" t="inlineStr"/>
-      <c r="N72" t="inlineStr"/>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>#</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>Brianna</t>
+        </is>
+      </c>
       <c r="O72" t="inlineStr"/>
       <c r="P72" t="inlineStr"/>
       <c r="Q72" t="inlineStr"/>

</xml_diff>

<commit_message>
check up to ten rows down for next store
</commit_message>
<xml_diff>
--- a/07-07-24 to 07-13-24 Milwaukee Schedule Copy.xlsx
+++ b/07-07-24 to 07-13-24 Milwaukee Schedule Copy.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y81"/>
+  <dimension ref="A1:Y85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2345,11 +2345,7 @@
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr">
-        <is>
-          <t>6:00 AM START</t>
-        </is>
-      </c>
+      <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
@@ -2396,11 +2392,7 @@
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr"/>
-      <c r="N35" t="inlineStr">
-        <is>
-          <t>DC5-FINANCIAL</t>
-        </is>
-      </c>
+      <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr"/>
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
@@ -2447,11 +2439,7 @@
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr"/>
-      <c r="N36" t="inlineStr">
-        <is>
-          <t>PIGGLY WIGGLY #142, SUSSEX</t>
-        </is>
-      </c>
+      <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
@@ -2500,7 +2488,7 @@
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr">
         <is>
-          <t>N63 W23735 MAIN ST</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
@@ -2551,7 +2539,7 @@
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr">
         <is>
-          <t>https://maps.app.goo.gl/UHB7SgmVy27KNfWS7</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
@@ -2614,7 +2602,7 @@
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr">
         <is>
-          <t>*FIRST INVENTORY WITH BADGER</t>
+          <t>PIGGLY WIGGLY #142, SUSSEX</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
@@ -2655,7 +2643,11 @@
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr"/>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>N63 W23735 MAIN ST</t>
+        </is>
+      </c>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr">
@@ -2717,21 +2709,13 @@
         </is>
       </c>
       <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
+      <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr">
         <is>
-          <t>Kim</t>
-        </is>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>Sante Fe available, Equip</t>
-        </is>
-      </c>
+          <t>https://maps.app.goo.gl/UHB7SgmVy27KNfWS7</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr">
         <is>
@@ -2788,14 +2772,10 @@
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>2)</t>
-        </is>
-      </c>
+      <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr">
         <is>
-          <t>Casey</t>
+          <t>*FIRST INVENTORY WITH BADGER</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
@@ -2847,16 +2827,8 @@
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>3)</t>
-        </is>
-      </c>
-      <c r="N43" t="inlineStr">
-        <is>
-          <t>DJ</t>
-        </is>
-      </c>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
@@ -2888,15 +2860,19 @@
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr">
         <is>
-          <t>4)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>Greg</t>
-        </is>
-      </c>
-      <c r="O44" t="inlineStr"/>
+          <t>Kim</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>Sante Fe available, Equip</t>
+        </is>
+      </c>
       <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr">
@@ -2931,12 +2907,12 @@
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr">
         <is>
-          <t>5)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>Jerry D</t>
+          <t>Casey</t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
@@ -2965,11 +2941,7 @@
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>5:15 AM MEET COLLEGE (SOUTHWEST)</t>
-        </is>
-      </c>
+      <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
       <c r="I46" t="inlineStr"/>
@@ -2982,12 +2954,12 @@
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="inlineStr">
         <is>
-          <t>6)</t>
+          <t>3)</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>DJ</t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
@@ -3016,11 +2988,7 @@
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>6:00 AM START</t>
-        </is>
-      </c>
+      <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr"/>
@@ -3037,12 +3005,12 @@
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr">
         <is>
-          <t>7)</t>
+          <t>4)</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Greg</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
@@ -3071,19 +3039,23 @@
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>DC5-FINANCIAL</t>
-        </is>
-      </c>
+      <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
       <c r="I48" t="inlineStr"/>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>5)</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>Jerry D</t>
+        </is>
+      </c>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
@@ -3110,19 +3082,23 @@
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>PIGGLY WIGGLY #209, KENOSHA</t>
-        </is>
-      </c>
+      <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
-      <c r="M49" t="inlineStr"/>
-      <c r="N49" t="inlineStr"/>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>6)</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>Katherine</t>
+        </is>
+      </c>
       <c r="O49" t="inlineStr"/>
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
@@ -3151,7 +3127,7 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>7600 PERSHING BLVD</t>
+          <t>5:15 AM MEET COLLEGE (SOUTHWEST)</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -3160,10 +3136,14 @@
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr"/>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>7)</t>
+        </is>
+      </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>4:15 AM OFFICE LEAVE TIME</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="O50" t="inlineStr"/>
@@ -3194,7 +3174,7 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/JzRgLG7fbbR2</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -3204,11 +3184,7 @@
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
       <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr">
-        <is>
-          <t>6:00 AM START</t>
-        </is>
-      </c>
+      <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
@@ -3237,7 +3213,7 @@
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t>4:30 am meet for Carlie/Trevor at Grafton Park n Ride</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -3247,11 +3223,7 @@
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
       <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr">
-        <is>
-          <t>DC5-FINANCIAL</t>
-        </is>
-      </c>
+      <c r="N52" t="inlineStr"/>
       <c r="O52" t="inlineStr"/>
       <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr"/>
@@ -3278,7 +3250,11 @@
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
-      <c r="F53" t="inlineStr"/>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>PIGGLY WIGGLY #209, KENOSHA</t>
+        </is>
+      </c>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr"/>
@@ -3288,7 +3264,7 @@
       <c r="M53" t="inlineStr"/>
       <c r="N53" t="inlineStr">
         <is>
-          <t>PIGGLY WIGGLY #038, MENASHA</t>
+          <t>4:15 AM OFFICE LEAVE TIME</t>
         </is>
       </c>
       <c r="O53" t="inlineStr"/>
@@ -3312,22 +3288,13 @@
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
+      <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Kim</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>Driver,
-Sante Fe, Equip</t>
-        </is>
-      </c>
+          <t>7600 PERSHING BLVD</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
       <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr"/>
@@ -3336,7 +3303,7 @@
       <c r="M54" t="inlineStr"/>
       <c r="N54" t="inlineStr">
         <is>
-          <t>1151 MIDWAY RD</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="O54" t="inlineStr"/>
@@ -3372,23 +3339,13 @@
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>2)</t>
-        </is>
-      </c>
+      <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Carlie</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>Driver,
-White Camry
-(w/ Trevor)</t>
-        </is>
-      </c>
+          <t>https://goo.gl/maps/JzRgLG7fbbR2</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr"/>
@@ -3397,7 +3354,7 @@
       <c r="M55" t="inlineStr"/>
       <c r="N55" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/ufFM5TycoD42</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="O55" t="inlineStr"/>
@@ -3425,14 +3382,10 @@
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>3)</t>
-        </is>
-      </c>
+      <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Joshua M</t>
+          <t>4:30 am meet for Carlie/Trevor at Grafton Park n Ride</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
@@ -3444,7 +3397,7 @@
       <c r="M56" t="inlineStr"/>
       <c r="N56" t="inlineStr">
         <is>
-          <t>LIQUOR &amp; SMALL RESETS-REMAPPED</t>
+          <t>PIGGLY WIGGLY #038, MENASHA</t>
         </is>
       </c>
       <c r="O56" t="inlineStr"/>
@@ -3484,16 +3437,8 @@
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>4)</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>Katherine</t>
-        </is>
-      </c>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr"/>
@@ -3503,7 +3448,7 @@
       <c r="M57" t="inlineStr"/>
       <c r="N57" t="inlineStr">
         <is>
-          <t>4:15 am meet for Carlie/Trevor at Grafton Park n Ride</t>
+          <t>1151 MIDWAY RD</t>
         </is>
       </c>
       <c r="O57" t="inlineStr"/>
@@ -3537,17 +3482,18 @@
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
         <is>
-          <t>5)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Nick</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>@ Store</t>
+          <t>Driver,
+Sante Fe, Equip</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
@@ -3558,7 +3504,7 @@
       <c r="M58" t="inlineStr"/>
       <c r="N58" t="inlineStr">
         <is>
-          <t>4:45 am meet at Slinger Piggly Wiggly (Lashaun/Carlie/Trevor)</t>
+          <t>https://goo.gl/maps/ufFM5TycoD42</t>
         </is>
       </c>
       <c r="O58" t="inlineStr"/>
@@ -3580,22 +3526,32 @@
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
         <is>
-          <t>6)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Sonia</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr"/>
+          <t>Carlie</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Driver,
+White Camry
+(w/ Trevor)</t>
+        </is>
+      </c>
       <c r="H59" t="inlineStr"/>
       <c r="I59" t="inlineStr"/>
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr"/>
       <c r="M59" t="inlineStr"/>
-      <c r="N59" t="inlineStr"/>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>LIQUOR &amp; SMALL RESETS-REMAPPED</t>
+        </is>
+      </c>
       <c r="O59" t="inlineStr"/>
       <c r="P59" t="inlineStr"/>
       <c r="Q59" t="inlineStr"/>
@@ -3619,12 +3575,12 @@
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
         <is>
-          <t>7)</t>
+          <t>3)</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Stephanie</t>
+          <t>Joshua M</t>
         </is>
       </c>
       <c r="G60" t="inlineStr"/>
@@ -3633,21 +3589,13 @@
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="inlineStr"/>
       <c r="L60" t="inlineStr"/>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
+      <c r="M60" t="inlineStr"/>
       <c r="N60" t="inlineStr">
         <is>
-          <t>Jeremiah</t>
-        </is>
-      </c>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>@ Store, Equip</t>
-        </is>
-      </c>
+          <t>4:15 am meet for Carlie/Trevor at Grafton Park n Ride</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr"/>
       <c r="P60" t="inlineStr"/>
       <c r="Q60" t="inlineStr"/>
       <c r="R60" t="inlineStr"/>
@@ -3670,39 +3618,27 @@
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr">
         <is>
-          <t>8)</t>
+          <t>4)</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Trevor</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>(w/ Carlie)</t>
-        </is>
-      </c>
+          <t>Katherine</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
       <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr"/>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>2)</t>
-        </is>
-      </c>
+      <c r="M61" t="inlineStr"/>
       <c r="N61" t="inlineStr">
         <is>
-          <t>Carlie</t>
-        </is>
-      </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>(w/ Trevor to Slinger)</t>
-        </is>
-      </c>
+          <t>4:45 am meet at Slinger Piggly Wiggly (Lashaun/Carlie/Trevor)</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr"/>
       <c r="P61" t="inlineStr"/>
       <c r="Q61" t="inlineStr"/>
       <c r="R61" t="inlineStr"/>
@@ -3721,36 +3657,27 @@
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr">
         <is>
-          <t>9)</t>
+          <t>5)</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Via</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr"/>
+          <t>Nick</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="H62" t="inlineStr"/>
       <c r="I62" t="inlineStr"/>
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr"/>
       <c r="L62" t="inlineStr"/>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>3)</t>
-        </is>
-      </c>
-      <c r="N62" t="inlineStr">
-        <is>
-          <t>Lashaun</t>
-        </is>
-      </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>Driver,
-Optima</t>
-        </is>
-      </c>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr"/>
+      <c r="O62" t="inlineStr"/>
       <c r="P62" t="inlineStr"/>
       <c r="Q62" t="inlineStr"/>
       <c r="R62" t="inlineStr"/>
@@ -3767,8 +3694,16 @@
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr"/>
-      <c r="E63" t="inlineStr"/>
-      <c r="F63" t="inlineStr"/>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>6)</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Sonia</t>
+        </is>
+      </c>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr"/>
@@ -3777,17 +3712,17 @@
       <c r="L63" t="inlineStr"/>
       <c r="M63" t="inlineStr">
         <is>
-          <t>4)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Jeremiah</t>
         </is>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>(w/ Carlie)</t>
+          <t>@ Store, Equip</t>
         </is>
       </c>
       <c r="P63" t="inlineStr"/>
@@ -3806,8 +3741,16 @@
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr"/>
-      <c r="F64" t="inlineStr"/>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>7)</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Stephanie</t>
+        </is>
+      </c>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
       <c r="I64" t="inlineStr"/>
@@ -3816,17 +3759,17 @@
       <c r="L64" t="inlineStr"/>
       <c r="M64" t="inlineStr">
         <is>
-          <t>5)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="N64" t="inlineStr">
         <is>
-          <t>Annette</t>
+          <t>Carlie</t>
         </is>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t xml:space="preserve">@ Store  </t>
+          <t>(w/ Trevor to Slinger)</t>
         </is>
       </c>
       <c r="P64" t="inlineStr"/>
@@ -3845,13 +3788,21 @@
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr"/>
-      <c r="E65" t="inlineStr"/>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>8)</t>
+        </is>
+      </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr"/>
+          <t>Trevor</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>(w/ Carlie)</t>
+        </is>
+      </c>
       <c r="H65" t="inlineStr"/>
       <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr"/>
@@ -3859,17 +3810,18 @@
       <c r="L65" t="inlineStr"/>
       <c r="M65" t="inlineStr">
         <is>
-          <t>6)</t>
+          <t>3)</t>
         </is>
       </c>
       <c r="N65" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Lashaun</t>
         </is>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t xml:space="preserve">@ Store  </t>
+          <t>Driver,
+Optima</t>
         </is>
       </c>
       <c r="P65" t="inlineStr"/>
@@ -3888,10 +3840,14 @@
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr"/>
-      <c r="E66" t="inlineStr"/>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>9)</t>
+        </is>
+      </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>Via</t>
         </is>
       </c>
       <c r="G66" t="inlineStr"/>
@@ -3902,17 +3858,17 @@
       <c r="L66" t="inlineStr"/>
       <c r="M66" t="inlineStr">
         <is>
-          <t>7)</t>
+          <t>4)</t>
         </is>
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>Jerry S</t>
+          <t>Trevor</t>
         </is>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t xml:space="preserve">@ Store  </t>
+          <t>(w/ Carlie)</t>
         </is>
       </c>
       <c r="P66" t="inlineStr"/>
@@ -3932,11 +3888,7 @@
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr"/>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>PIGGLY WIGGLY #208, DELAVAN</t>
-        </is>
-      </c>
+      <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr"/>
@@ -3945,12 +3897,12 @@
       <c r="L67" t="inlineStr"/>
       <c r="M67" t="inlineStr">
         <is>
-          <t>8)</t>
+          <t>5)</t>
         </is>
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>Kirsten</t>
+          <t>Annette</t>
         </is>
       </c>
       <c r="O67" t="inlineStr">
@@ -3975,11 +3927,7 @@
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr"/>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>1414 E GENEVA ST</t>
-        </is>
-      </c>
+      <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr"/>
@@ -3988,12 +3936,12 @@
       <c r="L68" t="inlineStr"/>
       <c r="M68" t="inlineStr">
         <is>
-          <t>9)</t>
+          <t>6)</t>
         </is>
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>Louisa</t>
+          <t>David</t>
         </is>
       </c>
       <c r="O68" t="inlineStr">
@@ -4020,7 +3968,7 @@
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/hixkUheCekD2</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="G69" t="inlineStr"/>
@@ -4031,12 +3979,12 @@
       <c r="L69" t="inlineStr"/>
       <c r="M69" t="inlineStr">
         <is>
-          <t>10)</t>
+          <t>7)</t>
         </is>
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>Michelle</t>
+          <t>Jerry S</t>
         </is>
       </c>
       <c r="O69" t="inlineStr">
@@ -4061,7 +4009,11 @@
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr"/>
-      <c r="F70" t="inlineStr"/>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>DC5-FINANCIAL</t>
+        </is>
+      </c>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr"/>
@@ -4070,12 +4022,12 @@
       <c r="L70" t="inlineStr"/>
       <c r="M70" t="inlineStr">
         <is>
-          <t>11)</t>
+          <t>8)</t>
         </is>
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>Serena</t>
+          <t>Kirsten</t>
         </is>
       </c>
       <c r="O70" t="inlineStr">
@@ -4099,21 +4051,13 @@
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
+      <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Nate</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>@ Store, Equip</t>
-        </is>
-      </c>
+          <t>PIGGLY WIGGLY #208, DELAVAN</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
       <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr"/>
@@ -4121,12 +4065,12 @@
       <c r="L71" t="inlineStr"/>
       <c r="M71" t="inlineStr">
         <is>
-          <t>12)</t>
+          <t>9)</t>
         </is>
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>Taya</t>
+          <t>Louisa</t>
         </is>
       </c>
       <c r="O71" t="inlineStr">
@@ -4150,21 +4094,13 @@
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>2)</t>
-        </is>
-      </c>
+      <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Anisha</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>@ Store</t>
-        </is>
-      </c>
+          <t>1414 E GENEVA ST</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr"/>
@@ -4172,17 +4108,17 @@
       <c r="L72" t="inlineStr"/>
       <c r="M72" t="inlineStr">
         <is>
-          <t>13)</t>
+          <t>10)</t>
         </is>
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>Leshaun</t>
+          <t>Michelle</t>
         </is>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>@ Store</t>
+          <t xml:space="preserve">@ Store  </t>
         </is>
       </c>
       <c r="P72" t="inlineStr"/>
@@ -4201,29 +4137,33 @@
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>3)</t>
-        </is>
-      </c>
+      <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Ashley P</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>@ Store</t>
-        </is>
-      </c>
+          <t>https://goo.gl/maps/hixkUheCekD2</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="inlineStr"/>
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr"/>
-      <c r="M73" t="inlineStr"/>
-      <c r="N73" t="inlineStr"/>
-      <c r="O73" t="inlineStr"/>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>11)</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>Serena</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">@ Store  </t>
+        </is>
+      </c>
       <c r="P73" t="inlineStr"/>
       <c r="Q73" t="inlineStr"/>
       <c r="R73" t="inlineStr"/>
@@ -4240,29 +4180,29 @@
       <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>4)</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>Joseph</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>@ Store</t>
-        </is>
-      </c>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr"/>
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr"/>
       <c r="L74" t="inlineStr"/>
-      <c r="M74" t="inlineStr"/>
-      <c r="N74" t="inlineStr"/>
-      <c r="O74" t="inlineStr"/>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>12)</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>Taya</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">@ Store  </t>
+        </is>
+      </c>
       <c r="P74" t="inlineStr"/>
       <c r="Q74" t="inlineStr"/>
       <c r="R74" t="inlineStr"/>
@@ -4281,17 +4221,17 @@
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr">
         <is>
-          <t>5)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Josh S</t>
+          <t>Nate</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>@ Store</t>
+          <t>@ Store, Equip</t>
         </is>
       </c>
       <c r="H75" t="inlineStr"/>
@@ -4299,9 +4239,21 @@
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr"/>
       <c r="L75" t="inlineStr"/>
-      <c r="M75" t="inlineStr"/>
-      <c r="N75" t="inlineStr"/>
-      <c r="O75" t="inlineStr"/>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>13)</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>Leshaun</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="P75" t="inlineStr"/>
       <c r="Q75" t="inlineStr"/>
       <c r="R75" t="inlineStr"/>
@@ -4320,12 +4272,12 @@
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr">
         <is>
-          <t>6)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Josie</t>
+          <t>Anisha</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -4359,12 +4311,12 @@
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr">
         <is>
-          <t>7)</t>
+          <t>3)</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Justin</t>
+          <t>Ashley P</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -4398,12 +4350,12 @@
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr">
         <is>
-          <t>8)</t>
+          <t>4)</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Lori</t>
+          <t>Joseph</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -4437,12 +4389,12 @@
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="inlineStr">
         <is>
-          <t>9)</t>
+          <t>5)</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Michael N</t>
+          <t>Josh S</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -4476,12 +4428,12 @@
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr">
         <is>
-          <t>10)</t>
+          <t>6)</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>Josie</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -4515,12 +4467,12 @@
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr">
         <is>
-          <t>11)</t>
+          <t>7)</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Wyatt</t>
+          <t>Justin</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -4547,6 +4499,162 @@
       <c r="X81" t="inlineStr"/>
       <c r="Y81" t="inlineStr"/>
     </row>
+    <row r="82">
+      <c r="A82" t="inlineStr"/>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>8)</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Lori</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr"/>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
+      <c r="K82" t="inlineStr"/>
+      <c r="L82" t="inlineStr"/>
+      <c r="M82" t="inlineStr"/>
+      <c r="N82" t="inlineStr"/>
+      <c r="O82" t="inlineStr"/>
+      <c r="P82" t="inlineStr"/>
+      <c r="Q82" t="inlineStr"/>
+      <c r="R82" t="inlineStr"/>
+      <c r="S82" t="inlineStr"/>
+      <c r="T82" t="inlineStr"/>
+      <c r="U82" t="inlineStr"/>
+      <c r="V82" t="inlineStr"/>
+      <c r="W82" t="inlineStr"/>
+      <c r="X82" t="inlineStr"/>
+      <c r="Y82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr"/>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr"/>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>9)</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Michael N</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr"/>
+      <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr"/>
+      <c r="K83" t="inlineStr"/>
+      <c r="L83" t="inlineStr"/>
+      <c r="M83" t="inlineStr"/>
+      <c r="N83" t="inlineStr"/>
+      <c r="O83" t="inlineStr"/>
+      <c r="P83" t="inlineStr"/>
+      <c r="Q83" t="inlineStr"/>
+      <c r="R83" t="inlineStr"/>
+      <c r="S83" t="inlineStr"/>
+      <c r="T83" t="inlineStr"/>
+      <c r="U83" t="inlineStr"/>
+      <c r="V83" t="inlineStr"/>
+      <c r="W83" t="inlineStr"/>
+      <c r="X83" t="inlineStr"/>
+      <c r="Y83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr"/>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr"/>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>10)</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Sarah</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr"/>
+      <c r="K84" t="inlineStr"/>
+      <c r="L84" t="inlineStr"/>
+      <c r="M84" t="inlineStr"/>
+      <c r="N84" t="inlineStr"/>
+      <c r="O84" t="inlineStr"/>
+      <c r="P84" t="inlineStr"/>
+      <c r="Q84" t="inlineStr"/>
+      <c r="R84" t="inlineStr"/>
+      <c r="S84" t="inlineStr"/>
+      <c r="T84" t="inlineStr"/>
+      <c r="U84" t="inlineStr"/>
+      <c r="V84" t="inlineStr"/>
+      <c r="W84" t="inlineStr"/>
+      <c r="X84" t="inlineStr"/>
+      <c r="Y84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr"/>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr"/>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>11)</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Wyatt</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr"/>
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr"/>
+      <c r="K85" t="inlineStr"/>
+      <c r="L85" t="inlineStr"/>
+      <c r="M85" t="inlineStr"/>
+      <c r="N85" t="inlineStr"/>
+      <c r="O85" t="inlineStr"/>
+      <c r="P85" t="inlineStr"/>
+      <c r="Q85" t="inlineStr"/>
+      <c r="R85" t="inlineStr"/>
+      <c r="S85" t="inlineStr"/>
+      <c r="T85" t="inlineStr"/>
+      <c r="U85" t="inlineStr"/>
+      <c r="V85" t="inlineStr"/>
+      <c r="W85" t="inlineStr"/>
+      <c r="X85" t="inlineStr"/>
+      <c r="Y85" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
don't display extra info when helping stores
</commit_message>
<xml_diff>
--- a/07-07-24 to 07-13-24 Milwaukee Schedule Copy.xlsx
+++ b/07-07-24 to 07-13-24 Milwaukee Schedule Copy.xlsx
@@ -1559,7 +1559,11 @@
           <t>Via</t>
         </is>
       </c>
-      <c r="O21" t="inlineStr"/>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>After Store</t>
+        </is>
+      </c>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr">
         <is>
@@ -3221,9 +3225,21 @@
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
-      <c r="M49" t="inlineStr"/>
-      <c r="N49" t="inlineStr"/>
-      <c r="O49" t="inlineStr"/>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>8)</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>Via</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>After</t>
+        </is>
+      </c>
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr">
@@ -4258,8 +4274,16 @@
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr"/>
       <c r="L72" t="inlineStr"/>
-      <c r="M72" t="inlineStr"/>
-      <c r="N72" t="inlineStr"/>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>12)</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>Via</t>
+        </is>
+      </c>
       <c r="O72" t="inlineStr"/>
       <c r="P72" t="inlineStr"/>
       <c r="Q72" t="inlineStr"/>

</xml_diff>